<commit_message>
add excel download /mylist, /otherslist
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/xls/shipreqdata.xlsx
+++ b/src/main/webapp/resources/xls/shipreqdata.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>LGIT P/N</t>
   </si>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -87,17 +83,120 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TESTPRJ002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발자시험용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>asdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>TESTPRJA</t>
   </si>
   <si>
+    <t>개발자테스트아이디</t>
+  </si>
+  <si>
+    <t>전장부품</t>
+  </si>
+  <si>
+    <t>출고담당자시험용</t>
+  </si>
+  <si>
+    <t>2FTS00096A</t>
+  </si>
+  <si>
+    <t>F6HF2G441AF46</t>
+  </si>
+  <si>
+    <t>TAIYO YUDEN</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2FTS00093A</t>
+  </si>
+  <si>
+    <t>B39242-B4346-P810</t>
+  </si>
+  <si>
+    <t>EPCOS AG</t>
+  </si>
+  <si>
     <t>2FTC00145A</t>
+  </si>
+  <si>
+    <t>DLU-2012-25GS1-A1-AT</t>
+  </si>
+  <si>
+    <t>MAGLAYERS</t>
+  </si>
+  <si>
+    <t>2FTP00015A</t>
+  </si>
+  <si>
+    <t>DPX165950DT-8126A1</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>2ICZ00186A</t>
+  </si>
+  <si>
+    <t>RFFM8800TR7</t>
+  </si>
+  <si>
+    <t>RFMD</t>
+  </si>
+  <si>
+    <t>2ICT00113A</t>
+  </si>
+  <si>
+    <t>AR6003XBC2B-R</t>
+  </si>
+  <si>
+    <t>QUALCOMM INCORPORATED</t>
+  </si>
+  <si>
+    <t>2OSR00012A</t>
+  </si>
+  <si>
+    <t>1ZCL26000AB0F</t>
+  </si>
+  <si>
+    <t>KDS</t>
+  </si>
+  <si>
+    <t>2CAC00801A</t>
+  </si>
+  <si>
+    <t>GRM033R71E471KA01D</t>
+  </si>
+  <si>
+    <t>MURATA ELEKTRONIK</t>
+  </si>
+  <si>
+    <t>2LL2N5BA11K-R</t>
+  </si>
+  <si>
+    <t>LQP03TN2N5B02D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <numFmts count="0"/>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +263,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF555555"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -214,7 +320,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -243,6 +349,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -577,13 +686,13 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="4" width="16.125" customWidth="1"/>
-    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="1" max="4" customWidth="true" width="16.125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="11.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75">
@@ -616,7 +725,7 @@
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -647,39 +756,319 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18">
-      <c r="A5" s="9" t="s">
-        <v>18</v>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>11</v>
-      </c>
-      <c r="J5">
-        <v>12</v>
-      </c>
-      <c r="K5">
-        <v>88</v>
+        <v>26</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.2130000591278076</v>
+      </c>
+      <c r="I5" t="n">
+        <v>530.0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.210999995470047</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3000.0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="n">
+        <v>351.1210021972656</v>
+      </c>
+      <c r="I7" t="n">
+        <v>4450.0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" t="n">
+        <v>53.21229934692383</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2260.0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.12309999763965607</v>
+      </c>
+      <c r="I9" t="n">
+        <v>768.0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.12399999797344208</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1275.0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.352400004863739</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2200.0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.15600000321865082</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1560.0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.12300000339746475</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4000.0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>